<commit_message>
Cambios en el formato.
</commit_message>
<xml_diff>
--- a/Documentos_proyecto/8.-MatrizDeRiesgos_v2.xlsx
+++ b/Documentos_proyecto/8.-MatrizDeRiesgos_v2.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Javeriana Cali\2016-2\Gran Escala\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Universidad\VII\Gran Escala\GranScala\Documentos_proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="989"/>
+    <workbookView xWindow="888" yWindow="0" windowWidth="20496" windowHeight="7536" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>Probabilidad</t>
   </si>
@@ -53,15 +53,9 @@
     <t>Manejo del Riesgo</t>
   </si>
   <si>
-    <t>Código del riesgo</t>
-  </si>
-  <si>
     <t>Reportado por</t>
   </si>
   <si>
-    <t>fecha de reporte</t>
-  </si>
-  <si>
     <t>Estado</t>
   </si>
   <si>
@@ -104,12 +98,6 @@
     <t>el proyecto se retrase</t>
   </si>
   <si>
-    <t>el no termino del proyecto en los plazos previstos</t>
-  </si>
-  <si>
-    <t>El equipo de trabajo tiene responsabilidades fuera del proyecto a las cuales estos no puede faltar</t>
-  </si>
-  <si>
     <t>Realizar una planificación con un holgura</t>
   </si>
   <si>
@@ -122,9 +110,6 @@
     <t>El poco tiempo para desarrollar cada modulo</t>
   </si>
   <si>
-    <t>que el producto no cumpla con la rapidez de respuesta esperada</t>
-  </si>
-  <si>
     <t>Al tratarse se una metodologia semi-SCRUM lo mas importante es que el producto este terminado por lo que la eficiencia esta presente pero no es el tema mas relevante</t>
   </si>
   <si>
@@ -134,9 +119,6 @@
     <t>Una nueva ley que establezca que los estudiantes van a recibir un subsidio para sus estudios profesionales</t>
   </si>
   <si>
-    <t>el producto no tenga ningún valor para la empresa de empaques</t>
-  </si>
-  <si>
     <t>Ampliar el mercado para poder ofrecer un servicio diferente a empresas que no sean del mismo sector con el fin de que supla una necesidad.</t>
   </si>
   <si>
@@ -155,9 +137,6 @@
     <t>los estudiantes no quieran trabajar en la empresa de empaques</t>
   </si>
   <si>
-    <t>que se dejen por fuera funcionalidades importantes e incumpliendo con los requerimientos</t>
-  </si>
-  <si>
     <t>Que una empresa esté desarrollando el mismo proyecto con más funcionalidades que las que vamos a desarrollar en el mismo límite de tiempo</t>
   </si>
   <si>
@@ -167,18 +146,12 @@
     <t>la empresa de empaques no esté interesada en nuestro producto</t>
   </si>
   <si>
-    <t>la cancelación o cambio del enfoque proyecto</t>
-  </si>
-  <si>
     <t>El desconocimiento de las tecnologías que se van a utilizar para desarrollar el proyecto por parte de los integrantes</t>
   </si>
   <si>
     <t>la curva de aprendizaje sea tan alta</t>
   </si>
   <si>
-    <t>el tiempo para desarrollar el proyecto no se cumpla</t>
-  </si>
-  <si>
     <t>Definir una propuesta de valor para el proyecto que se diferencie de cualquier producto en el mercado.</t>
   </si>
   <si>
@@ -186,12 +159,39 @@
   </si>
   <si>
     <t>Delegar responsabilidades a parejas.</t>
+  </si>
+  <si>
+    <t>Fecha de reporte</t>
+  </si>
+  <si>
+    <t>El equipo de trabajo tiene responsabilidades fuera del proyecto a las cuales estos no puede faltar.</t>
+  </si>
+  <si>
+    <t>el no termino del proyecto en los plazos previstos.</t>
+  </si>
+  <si>
+    <t>que el producto no cumpla con la rapidez de respuesta esperada.</t>
+  </si>
+  <si>
+    <t>el producto no tenga ningún valor para la empresa de empaques.</t>
+  </si>
+  <si>
+    <t>que se dejen por fuera funcionalidades importantes e incumpliendo con los requerimientos.</t>
+  </si>
+  <si>
+    <t>la cancelación o cambio del enfoque proyecto.</t>
+  </si>
+  <si>
+    <t>el tiempo para desarrollar el proyecto no se cumpla.</t>
+  </si>
+  <si>
+    <t>Código</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -324,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -354,7 +354,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,10 +370,27 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,30 +850,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375"/>
-    <col min="2" max="2" width="18.140625"/>
-    <col min="3" max="3" width="18"/>
-    <col min="4" max="4" width="9.85546875"/>
-    <col min="5" max="5" width="15.42578125"/>
-    <col min="6" max="6" width="19"/>
-    <col min="7" max="7" width="18.5703125"/>
-    <col min="8" max="8" width="25.85546875"/>
-    <col min="9" max="9" width="26"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625"/>
-    <col min="13" max="13" width="30.7109375"/>
-    <col min="14" max="14" width="18.140625"/>
-    <col min="15" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875"/>
+    <col min="5" max="5" width="15.44140625"/>
+    <col min="6" max="6" width="40.77734375" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="8" max="8" width="32.88671875" customWidth="1"/>
+    <col min="9" max="9" width="40.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375"/>
+    <col min="13" max="13" width="46.88671875" customWidth="1"/>
+    <col min="14" max="14" width="18.109375"/>
+    <col min="15" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -872,7 +892,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -897,7 +917,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -909,7 +929,7 @@
       <c r="I3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="19">
         <v>7</v>
       </c>
       <c r="K3" s="8">
@@ -922,7 +942,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -937,7 +957,7 @@
       <c r="J4" s="9">
         <v>9</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="20">
         <v>8</v>
       </c>
       <c r="L4" s="8">
@@ -947,7 +967,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -972,7 +992,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -989,7 +1009,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1006,7 +1026,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1023,57 +1043,57 @@
       <c r="N8" s="2"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="22" t="s">
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="23" t="s">
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="N9" s="23"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N9" s="24"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="C10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="F10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="G10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="H10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="I10" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="J10" s="13" t="s">
         <v>0</v>
@@ -1082,278 +1102,278 @@
         <v>4</v>
       </c>
       <c r="L10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="14" t="s">
+    </row>
+    <row r="11" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A11" s="30">
+        <v>1</v>
+      </c>
+      <c r="B11" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="C11" s="31">
+        <v>42619</v>
+      </c>
+      <c r="D11" s="30" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="15">
+      <c r="E11" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="19">
-        <v>42619</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="17" t="s">
+      <c r="K11" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="K11" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L11" s="17">
+      <c r="L11" s="28">
         <f t="shared" ref="L11:L20" si="0">IF(AND(J11=$I$2,K11=$J$5),$J$2,IF(AND(J11=$I$2,K11=$K$5),$K$2,IF(AND(J11=$I$2,K11=$L$5),$L$2,IF(AND(J11=$I$3,K11=$J$5),$J$3,IF(AND(J11=$I$3,K11=$K$5),$K$3,IF(AND(J11=$I$3,K11=$L$5),$L$3,IF(AND(J11=$I$4,K11=$J$5),$J$4,IF(AND(J11=$I$4,K11=$K$5),$K$4,IF(AND(J11=$I$4,K11=$L$5),$L$4,0)))))))))</f>
         <v>1</v>
       </c>
-      <c r="M11" s="18" t="s">
+      <c r="M11" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="30">
+        <v>2</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="31">
+        <v>42619</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="15">
+      <c r="J12" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="19">
-        <v>42619</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="L12" s="17">
+      <c r="L12" s="28">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="M12" s="18" t="s">
-        <v>34</v>
+      <c r="M12" s="27" t="s">
+        <v>29</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A13" s="30">
         <v>3</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="19">
+      <c r="B13" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="31">
         <v>42620</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="15" t="s">
+      <c r="D13" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="16" t="s">
+      <c r="G13" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17" t="s">
+      <c r="H13" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="26"/>
+      <c r="J13" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="28">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M13" s="18" t="s">
-        <v>37</v>
+      <c r="M13" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="30">
         <v>4</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="19">
+      <c r="B14" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="31">
         <v>42624</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="17" t="s">
+      <c r="D14" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14" s="26"/>
+      <c r="J14" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="L14" s="17">
+      <c r="L14" s="28">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="M14" s="18" t="s">
-        <v>53</v>
+      <c r="M14" s="27" t="s">
+        <v>44</v>
       </c>
       <c r="N14" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="30">
+        <v>5</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="31">
+        <v>42624</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="26" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="15">
-        <v>5</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="19">
-        <v>42624</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17" t="s">
+      <c r="H15" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="26"/>
+      <c r="J15" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="L15" s="17">
+      <c r="L15" s="28">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M15" s="18" t="s">
-        <v>51</v>
+      <c r="M15" s="27" t="s">
+        <v>42</v>
       </c>
       <c r="N15" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="30">
         <v>6</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="19">
+      <c r="B16" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="31">
         <v>42624</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17" t="s">
+      <c r="D16" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="26"/>
+      <c r="J16" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="17" t="s">
+      <c r="K16" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="28">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="M16" s="18" t="s">
-        <v>52</v>
+      <c r="M16" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="N16" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -1365,14 +1385,11 @@
       <c r="I17" s="16"/>
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
-      <c r="L17" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="18"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="25"/>
       <c r="N17" s="18"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -1384,14 +1401,11 @@
       <c r="I18" s="16"/>
       <c r="J18" s="17"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="18"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="25"/>
       <c r="N18" s="18"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -1403,14 +1417,11 @@
       <c r="I19" s="16"/>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="18"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="25"/>
       <c r="N19" s="18"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -1422,14 +1433,11 @@
       <c r="I20" s="16"/>
       <c r="J20" s="17"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="18"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="25"/>
       <c r="N20" s="18"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
@@ -1442,10 +1450,10 @@
       <c r="J21" s="17"/>
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
-      <c r="M21" s="18"/>
+      <c r="M21" s="25"/>
       <c r="N21" s="18"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -1458,10 +1466,10 @@
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17"/>
-      <c r="M22" s="18"/>
+      <c r="M22" s="25"/>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -1474,10 +1482,10 @@
       <c r="J23" s="17"/>
       <c r="K23" s="17"/>
       <c r="L23" s="17"/>
-      <c r="M23" s="18"/>
+      <c r="M23" s="25"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -1490,10 +1498,10 @@
       <c r="J24" s="17"/>
       <c r="K24" s="17"/>
       <c r="L24" s="17"/>
-      <c r="M24" s="18"/>
+      <c r="M24" s="25"/>
       <c r="N24" s="18"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -1506,10 +1514,10 @@
       <c r="J25" s="17"/>
       <c r="K25" s="17"/>
       <c r="L25" s="17"/>
-      <c r="M25" s="18"/>
+      <c r="M25" s="25"/>
       <c r="N25" s="18"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -1522,10 +1530,10 @@
       <c r="J26" s="17"/>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
-      <c r="M26" s="18"/>
+      <c r="M26" s="25"/>
       <c r="N26" s="18"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -1538,10 +1546,10 @@
       <c r="J27" s="17"/>
       <c r="K27" s="17"/>
       <c r="L27" s="17"/>
-      <c r="M27" s="18"/>
+      <c r="M27" s="25"/>
       <c r="N27" s="18"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1554,10 +1562,10 @@
       <c r="J28" s="17"/>
       <c r="K28" s="17"/>
       <c r="L28" s="17"/>
-      <c r="M28" s="18"/>
+      <c r="M28" s="25"/>
       <c r="N28" s="18"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1570,7 +1578,7 @@
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
       <c r="L29" s="17"/>
-      <c r="M29" s="18"/>
+      <c r="M29" s="25"/>
       <c r="N29" s="18"/>
     </row>
   </sheetData>

</xml_diff>